<commit_message>
Filter delivery points by EV
</commit_message>
<xml_diff>
--- a/data/37-intersection map.xlsx
+++ b/data/37-intersection map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80edabada1d31728/FolderSync/University/TFM EV Routing/A Routing Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99BF1457-DDE1-47DD-A50A-ADBD7D6FA2B3}"/>
+  <xr:revisionPtr revIDLastSave="365" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91614A49-F30F-48EA-A8AD-DC4A312A0EE6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unindexed" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="sDeliveryPoints" sheetId="1" r:id="rId4"/>
     <sheet name="sChargingStations" sheetId="2" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">sDeliveryPoints!$A$1:$E$15</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>pDelayPenalty [$/h]</t>
   </si>
@@ -152,12 +155,15 @@
   <si>
     <t>pDestinationIntersection</t>
   </si>
+  <si>
+    <t>EV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +194,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,11 +228,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,6 +251,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -665,7 +691,7 @@
       </c>
       <c r="J2" s="2">
         <f>VLOOKUP($F2,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K2">
         <f>VLOOKUP($F2,sPathTypes!$A:$I,9,FALSE)</f>
@@ -706,7 +732,7 @@
       </c>
       <c r="J3" s="2">
         <f>VLOOKUP($F3,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K3">
         <f>VLOOKUP($F3,sPathTypes!$A:$I,9,FALSE)</f>
@@ -747,7 +773,7 @@
       </c>
       <c r="J4" s="2">
         <f>VLOOKUP($F4,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K4">
         <f>VLOOKUP($F4,sPathTypes!$A:$I,9,FALSE)</f>
@@ -788,7 +814,7 @@
       </c>
       <c r="J5" s="2">
         <f>VLOOKUP($F5,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K5">
         <f>VLOOKUP($F5,sPathTypes!$A:$I,9,FALSE)</f>
@@ -829,7 +855,7 @@
       </c>
       <c r="J6" s="2">
         <f>VLOOKUP($F6,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K6">
         <f>VLOOKUP($F6,sPathTypes!$A:$I,9,FALSE)</f>
@@ -870,7 +896,7 @@
       </c>
       <c r="J7" s="2">
         <f>VLOOKUP($F7,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K7">
         <f>VLOOKUP($F7,sPathTypes!$A:$I,9,FALSE)</f>
@@ -911,7 +937,7 @@
       </c>
       <c r="J8" s="2">
         <f>VLOOKUP($F8,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K8">
         <f>VLOOKUP($F8,sPathTypes!$A:$I,9,FALSE)</f>
@@ -952,7 +978,7 @@
       </c>
       <c r="J9" s="2">
         <f>VLOOKUP($F9,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K9">
         <f>VLOOKUP($F9,sPathTypes!$A:$I,9,FALSE)</f>
@@ -993,7 +1019,7 @@
       </c>
       <c r="J10" s="2">
         <f>VLOOKUP($F10,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K10">
         <f>VLOOKUP($F10,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1034,7 +1060,7 @@
       </c>
       <c r="J11" s="2">
         <f>VLOOKUP($F11,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K11">
         <f>VLOOKUP($F11,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1075,7 +1101,7 @@
       </c>
       <c r="J12" s="2">
         <f>VLOOKUP($F12,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K12">
         <f>VLOOKUP($F12,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1116,7 +1142,7 @@
       </c>
       <c r="J13" s="2">
         <f>VLOOKUP($F13,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K13">
         <f>VLOOKUP($F13,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1157,7 +1183,7 @@
       </c>
       <c r="J14" s="2">
         <f>VLOOKUP($F14,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K14">
         <f>VLOOKUP($F14,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1198,7 +1224,7 @@
       </c>
       <c r="J15" s="2">
         <f>VLOOKUP($F15,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K15">
         <f>VLOOKUP($F15,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1239,7 +1265,7 @@
       </c>
       <c r="J16" s="2">
         <f>VLOOKUP($F16,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K16">
         <f>VLOOKUP($F16,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1280,7 +1306,7 @@
       </c>
       <c r="J17" s="2">
         <f>VLOOKUP($F17,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K17">
         <f>VLOOKUP($F17,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1321,7 +1347,7 @@
       </c>
       <c r="J18" s="2">
         <f>VLOOKUP($F18,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K18">
         <f>VLOOKUP($F18,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1362,7 +1388,7 @@
       </c>
       <c r="J19" s="2">
         <f>VLOOKUP($F19,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K19">
         <f>VLOOKUP($F19,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1403,7 +1429,7 @@
       </c>
       <c r="J20" s="2">
         <f>VLOOKUP($F20,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K20">
         <f>VLOOKUP($F20,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1444,7 +1470,7 @@
       </c>
       <c r="J21" s="2">
         <f>VLOOKUP($F21,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K21">
         <f>VLOOKUP($F21,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1485,7 +1511,7 @@
       </c>
       <c r="J22" s="2">
         <f>VLOOKUP($F22,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K22">
         <f>VLOOKUP($F22,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1526,7 +1552,7 @@
       </c>
       <c r="J23" s="2">
         <f>VLOOKUP($F23,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K23">
         <f>VLOOKUP($F23,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1567,7 +1593,7 @@
       </c>
       <c r="J24" s="2">
         <f>VLOOKUP($F24,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K24">
         <f>VLOOKUP($F24,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1608,7 +1634,7 @@
       </c>
       <c r="J25" s="2">
         <f>VLOOKUP($F25,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K25">
         <f>VLOOKUP($F25,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1649,7 +1675,7 @@
       </c>
       <c r="J26" s="2">
         <f>VLOOKUP($F26,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K26">
         <f>VLOOKUP($F26,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1690,7 +1716,7 @@
       </c>
       <c r="J27" s="2">
         <f>VLOOKUP($F27,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K27">
         <f>VLOOKUP($F27,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1731,7 +1757,7 @@
       </c>
       <c r="J28" s="2">
         <f>VLOOKUP($F28,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K28">
         <f>VLOOKUP($F28,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1772,7 +1798,7 @@
       </c>
       <c r="J29" s="2">
         <f>VLOOKUP($F29,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K29">
         <f>VLOOKUP($F29,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1813,7 +1839,7 @@
       </c>
       <c r="J30" s="2">
         <f>VLOOKUP($F30,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K30">
         <f>VLOOKUP($F30,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1854,7 +1880,7 @@
       </c>
       <c r="J31" s="2">
         <f>VLOOKUP($F31,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K31">
         <f>VLOOKUP($F31,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1895,7 +1921,7 @@
       </c>
       <c r="J32" s="2">
         <f>VLOOKUP($F32,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K32">
         <f>VLOOKUP($F32,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1936,7 +1962,7 @@
       </c>
       <c r="J33" s="2">
         <f>VLOOKUP($F33,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K33">
         <f>VLOOKUP($F33,sPathTypes!$A:$I,9,FALSE)</f>
@@ -1977,7 +2003,7 @@
       </c>
       <c r="J34" s="2">
         <f>VLOOKUP($F34,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K34">
         <f>VLOOKUP($F34,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2018,7 +2044,7 @@
       </c>
       <c r="J35" s="2">
         <f>VLOOKUP($F35,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K35">
         <f>VLOOKUP($F35,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2059,7 +2085,7 @@
       </c>
       <c r="J36" s="2">
         <f>VLOOKUP($F36,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K36">
         <f>VLOOKUP($F36,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2100,7 +2126,7 @@
       </c>
       <c r="J37" s="2">
         <f>VLOOKUP($F37,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K37">
         <f>VLOOKUP($F37,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2141,7 +2167,7 @@
       </c>
       <c r="J38" s="2">
         <f>VLOOKUP($F38,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K38">
         <f>VLOOKUP($F38,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2182,7 +2208,7 @@
       </c>
       <c r="J39" s="2">
         <f>VLOOKUP($F39,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K39">
         <f>VLOOKUP($F39,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2223,7 +2249,7 @@
       </c>
       <c r="J40" s="2">
         <f>VLOOKUP($F40,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K40">
         <f>VLOOKUP($F40,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2264,7 +2290,7 @@
       </c>
       <c r="J41" s="2">
         <f>VLOOKUP($F41,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K41">
         <f>VLOOKUP($F41,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2305,7 +2331,7 @@
       </c>
       <c r="J42" s="2">
         <f>VLOOKUP($F42,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K42">
         <f>VLOOKUP($F42,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2346,7 +2372,7 @@
       </c>
       <c r="J43" s="2">
         <f>VLOOKUP($F43,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K43">
         <f>VLOOKUP($F43,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2387,7 +2413,7 @@
       </c>
       <c r="J44" s="2">
         <f>VLOOKUP($F44,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K44">
         <f>VLOOKUP($F44,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2428,7 +2454,7 @@
       </c>
       <c r="J45" s="2">
         <f>VLOOKUP($F45,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K45">
         <f>VLOOKUP($F45,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2469,7 +2495,7 @@
       </c>
       <c r="J46" s="2">
         <f>VLOOKUP($F46,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K46">
         <f>VLOOKUP($F46,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2510,7 +2536,7 @@
       </c>
       <c r="J47" s="2">
         <f>VLOOKUP($F47,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K47">
         <f>VLOOKUP($F47,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2551,7 +2577,7 @@
       </c>
       <c r="J48" s="2">
         <f>VLOOKUP($F48,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K48">
         <f>VLOOKUP($F48,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2592,7 +2618,7 @@
       </c>
       <c r="J49" s="2">
         <f>VLOOKUP($F49,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K49">
         <f>VLOOKUP($F49,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2633,7 +2659,7 @@
       </c>
       <c r="J50" s="2">
         <f>VLOOKUP($F50,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K50">
         <f>VLOOKUP($F50,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2674,7 +2700,7 @@
       </c>
       <c r="J51" s="2">
         <f>VLOOKUP($F51,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K51">
         <f>VLOOKUP($F51,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2715,7 +2741,7 @@
       </c>
       <c r="J52" s="2">
         <f>VLOOKUP($F52,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K52">
         <f>VLOOKUP($F52,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2756,7 +2782,7 @@
       </c>
       <c r="J53" s="2">
         <f>VLOOKUP($F53,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K53">
         <f>VLOOKUP($F53,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2797,7 +2823,7 @@
       </c>
       <c r="J54" s="2">
         <f>VLOOKUP($F54,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K54">
         <f>VLOOKUP($F54,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2838,7 +2864,7 @@
       </c>
       <c r="J55" s="2">
         <f>VLOOKUP($F55,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K55">
         <f>VLOOKUP($F55,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2879,7 +2905,7 @@
       </c>
       <c r="J56" s="2">
         <f>VLOOKUP($F56,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K56">
         <f>VLOOKUP($F56,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2920,7 +2946,7 @@
       </c>
       <c r="J57" s="2">
         <f>VLOOKUP($F57,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K57">
         <f>VLOOKUP($F57,sPathTypes!$A:$I,9,FALSE)</f>
@@ -2961,7 +2987,7 @@
       </c>
       <c r="J58" s="2">
         <f>VLOOKUP($F58,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>319.44</v>
+        <v>7.3019999999999996</v>
       </c>
       <c r="K58">
         <f>VLOOKUP($F58,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3002,7 +3028,7 @@
       </c>
       <c r="J59" s="2">
         <f>VLOOKUP($F59,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K59">
         <f>VLOOKUP($F59,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3043,7 +3069,7 @@
       </c>
       <c r="J60" s="2">
         <f>VLOOKUP($F60,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K60">
         <f>VLOOKUP($F60,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3084,7 +3110,7 @@
       </c>
       <c r="J61" s="2">
         <f>VLOOKUP($F61,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K61">
         <f>VLOOKUP($F61,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3125,7 +3151,7 @@
       </c>
       <c r="J62" s="2">
         <f>VLOOKUP($F62,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K62">
         <f>VLOOKUP($F62,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3166,7 +3192,7 @@
       </c>
       <c r="J63" s="2">
         <f>VLOOKUP($F63,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K63">
         <f>VLOOKUP($F63,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3207,7 +3233,7 @@
       </c>
       <c r="J64" s="2">
         <f>VLOOKUP($F64,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K64">
         <f>VLOOKUP($F64,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3248,7 +3274,7 @@
       </c>
       <c r="J65" s="2">
         <f>VLOOKUP($F65,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K65">
         <f>VLOOKUP($F65,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3289,7 +3315,7 @@
       </c>
       <c r="J66" s="2">
         <f>VLOOKUP($F66,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K66">
         <f>VLOOKUP($F66,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3330,7 +3356,7 @@
       </c>
       <c r="J67" s="2">
         <f>VLOOKUP($F67,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K67">
         <f>VLOOKUP($F67,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3371,7 +3397,7 @@
       </c>
       <c r="J68" s="2">
         <f>VLOOKUP($F68,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K68">
         <f>VLOOKUP($F68,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3412,7 +3438,7 @@
       </c>
       <c r="J69" s="2">
         <f>VLOOKUP($F69,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K69">
         <f>VLOOKUP($F69,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3453,7 +3479,7 @@
       </c>
       <c r="J70" s="2">
         <f>VLOOKUP($F70,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K70">
         <f>VLOOKUP($F70,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3494,7 +3520,7 @@
       </c>
       <c r="J71" s="2">
         <f>VLOOKUP($F71,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K71">
         <f>VLOOKUP($F71,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3535,7 +3561,7 @@
       </c>
       <c r="J72" s="2">
         <f>VLOOKUP($F72,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K72">
         <f>VLOOKUP($F72,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3576,7 +3602,7 @@
       </c>
       <c r="J73" s="2">
         <f>VLOOKUP($F73,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K73">
         <f>VLOOKUP($F73,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3617,7 +3643,7 @@
       </c>
       <c r="J74" s="2">
         <f>VLOOKUP($F74,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K74">
         <f>VLOOKUP($F74,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3658,7 +3684,7 @@
       </c>
       <c r="J75" s="2">
         <f>VLOOKUP($F75,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K75">
         <f>VLOOKUP($F75,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3699,7 +3725,7 @@
       </c>
       <c r="J76" s="2">
         <f>VLOOKUP($F76,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>555.66</v>
+        <v>15.19</v>
       </c>
       <c r="K76">
         <f>VLOOKUP($F76,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3740,7 +3766,7 @@
       </c>
       <c r="J77" s="2">
         <f>VLOOKUP($F77,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K77">
         <f>VLOOKUP($F77,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3781,7 +3807,7 @@
       </c>
       <c r="J78" s="2">
         <f>VLOOKUP($F78,sPathTypes!$A:$I,8,FALSE)</f>
-        <v>182.13</v>
+        <v>4.444</v>
       </c>
       <c r="K78">
         <f>VLOOKUP($F78,sPathTypes!$A:$I,9,FALSE)</f>
@@ -3798,7 +3824,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3810,7 +3836,7 @@
     <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3836,7 +3862,7 @@
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3867,8 +3893,8 @@
         <f>(B2+D2)/1000</f>
         <v>5.8450000000000002E-2</v>
       </c>
-      <c r="H2" s="2">
-        <v>182.13</v>
+      <c r="H2" s="5">
+        <v>4.444</v>
       </c>
       <c r="I2">
         <v>2.24E-2</v>
@@ -3898,8 +3924,8 @@
         <f t="shared" ref="G3:G4" si="0">(B3+D3)/1000</f>
         <v>0.16238</v>
       </c>
-      <c r="H3" s="2">
-        <v>319.44</v>
+      <c r="H3" s="5">
+        <v>7.3019999999999996</v>
       </c>
       <c r="I3">
         <v>6.2399999999999997E-2</v>
@@ -3929,8 +3955,8 @@
         <f t="shared" si="0"/>
         <v>0.41567999999999999</v>
       </c>
-      <c r="H4" s="2">
-        <v>555.66</v>
+      <c r="H4" s="5">
+        <v>15.19</v>
       </c>
       <c r="I4">
         <v>0.16</v>
@@ -3943,147 +3969,279 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.25</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>24</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.25</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>24</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="C6">
         <v>0.25</v>
       </c>
-      <c r="C4">
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="E6">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
         <v>19</v>
       </c>
-      <c r="B5">
+      <c r="C8">
         <v>0.25</v>
       </c>
-      <c r="C5">
+      <c r="D8">
         <v>24</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="C9">
         <v>0.25</v>
       </c>
-      <c r="C6">
+      <c r="D9">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
         <v>27</v>
       </c>
-      <c r="B7">
+      <c r="C12">
         <v>0.25</v>
       </c>
-      <c r="C7">
+      <c r="D12">
         <v>24</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
         <v>29</v>
       </c>
-      <c r="B8">
+      <c r="C13">
         <v>0.25</v>
       </c>
-      <c r="C8">
+      <c r="D13">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="E13">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>0.25</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
         <v>35</v>
       </c>
-      <c r="B9">
+      <c r="C15">
         <v>0.25</v>
       </c>
-      <c r="C9">
+      <c r="D15">
         <v>24</v>
       </c>
-      <c r="D9">
+      <c r="E15">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E15" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4092,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918358E4-BA70-40E6-8885-148266F68FC9}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4102,8 +4260,8 @@
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4120,10 +4278,10 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4140,11 +4298,11 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
+      <c r="E2" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -4160,11 +4318,11 @@
       <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
+      <c r="E3" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -4180,11 +4338,11 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
+      <c r="E4" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.96</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4200,11 +4358,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
+      <c r="E5" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4220,11 +4378,11 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
+      <c r="E6" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made delivery points more balanced
</commit_message>
<xml_diff>
--- a/data/37-intersection map.xlsx
+++ b/data/37-intersection map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80edabada1d31728/FolderSync/University/TFM EV Routing/A Routing Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91614A49-F30F-48EA-A8AD-DC4A312A0EE6}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95E15225-EDE0-4BF0-BD09-16C4CDD36191}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3972,12 +3972,12 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -4012,10 +4012,10 @@
         <v>0.25</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -4046,10 +4046,10 @@
         <v>0.25</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -4114,10 +4114,10 @@
         <v>0.25</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -4200,10 +4200,10 @@
         <v>0.25</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added starting (24) and ending (38) points
</commit_message>
<xml_diff>
--- a/data/37-intersection map.xlsx
+++ b/data/37-intersection map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80edabada1d31728/FolderSync/University/TFM EV Routing/A Routing Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="378" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95E15225-EDE0-4BF0-BD09-16C4CDD36191}"/>
+  <xr:revisionPtr revIDLastSave="421" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFD3368F-712B-478B-9A6C-9EF0F0E689B5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unindexed" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">sDeliveryPoints!$A$1:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">sPaths!$A$1:$K$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>pDelayPenalty [$/h]</t>
   </si>
@@ -158,6 +159,12 @@
   <si>
     <t>EV</t>
   </si>
+  <si>
+    <t>pStartingPoint</t>
+  </si>
+  <si>
+    <t>pEndingPoint</t>
+  </si>
 </sst>
 </file>
 
@@ -167,13 +174,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,7 +189,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,12 +202,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,11 +237,11 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -520,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597D70E4-2172-494A-AB5D-BB966B7F274D}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,6 +602,22 @@
         <v>24</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="6">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -602,9 +625,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C34D7CB-5337-4A22-B32E-222A13B8F8D6}">
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -617,7 +642,7 @@
     <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.77734375" customWidth="1"/>
   </cols>
@@ -650,7 +675,7 @@
       <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -689,7 +714,7 @@
         <f>C2-H2</f>
         <v>7.3376200000000003</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="4">
         <f>VLOOKUP($F2,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -730,7 +755,7 @@
         <f t="shared" ref="I3:I66" si="1">C3-H3</f>
         <v>9.8376199999999994</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <f>VLOOKUP($F3,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -771,7 +796,7 @@
         <f t="shared" si="1"/>
         <v>10.941549999999999</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <f>VLOOKUP($F4,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -812,7 +837,7 @@
         <f t="shared" si="1"/>
         <v>9.9415499999999994</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <f>VLOOKUP($F5,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -853,7 +878,7 @@
         <f t="shared" si="1"/>
         <v>1.1415500000000001</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="4">
         <f>VLOOKUP($F6,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -894,7 +919,7 @@
         <f t="shared" si="1"/>
         <v>6.4415500000000003</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <f>VLOOKUP($F7,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -935,7 +960,7 @@
         <f t="shared" si="1"/>
         <v>2.9415499999999999</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="4">
         <f>VLOOKUP($F8,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -976,7 +1001,7 @@
         <f t="shared" si="1"/>
         <v>4.58432</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="4">
         <f>VLOOKUP($F9,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -1017,7 +1042,7 @@
         <f t="shared" si="1"/>
         <v>6.4415500000000003</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="4">
         <f>VLOOKUP($F10,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1058,7 +1083,7 @@
         <f t="shared" si="1"/>
         <v>11.837619999999999</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="4">
         <f>VLOOKUP($F11,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -1099,7 +1124,7 @@
         <f t="shared" si="1"/>
         <v>5.58432</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="4">
         <f>VLOOKUP($F12,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -1140,7 +1165,7 @@
         <f t="shared" si="1"/>
         <v>3.9415499999999999</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="4">
         <f>VLOOKUP($F13,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1181,7 +1206,7 @@
         <f t="shared" si="1"/>
         <v>3.9415499999999999</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="4">
         <f>VLOOKUP($F14,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1222,7 +1247,7 @@
         <f t="shared" si="1"/>
         <v>7.9415500000000003</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="4">
         <f>VLOOKUP($F15,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1263,7 +1288,7 @@
         <f t="shared" si="1"/>
         <v>9.4415499999999994</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="4">
         <f>VLOOKUP($F16,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1304,7 +1329,7 @@
         <f t="shared" si="1"/>
         <v>4.9415500000000003</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="4">
         <f>VLOOKUP($F17,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1345,7 +1370,7 @@
         <f t="shared" si="1"/>
         <v>14.941549999999999</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="4">
         <f>VLOOKUP($F18,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1386,7 +1411,7 @@
         <f t="shared" si="1"/>
         <v>12.941549999999999</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="4">
         <f>VLOOKUP($F19,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1427,7 +1452,7 @@
         <f t="shared" si="1"/>
         <v>3.4415499999999999</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="4">
         <f>VLOOKUP($F20,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1468,7 +1493,7 @@
         <f t="shared" si="1"/>
         <v>7.4415500000000003</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="4">
         <f>VLOOKUP($F21,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1509,7 +1534,7 @@
         <f t="shared" si="1"/>
         <v>4.8376200000000003</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="4">
         <f>VLOOKUP($F22,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -1550,7 +1575,7 @@
         <f t="shared" si="1"/>
         <v>6.4415500000000003</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="4">
         <f>VLOOKUP($F23,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1591,7 +1616,7 @@
         <f t="shared" si="1"/>
         <v>13.58432</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="4">
         <f>VLOOKUP($F24,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -1632,7 +1657,7 @@
         <f t="shared" si="1"/>
         <v>5.9415500000000003</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="4">
         <f>VLOOKUP($F25,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1673,7 +1698,7 @@
         <f t="shared" si="1"/>
         <v>7.4415500000000003</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="4">
         <f>VLOOKUP($F26,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1714,7 +1739,7 @@
         <f t="shared" si="1"/>
         <v>5.9415500000000003</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="4">
         <f>VLOOKUP($F27,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1755,7 +1780,7 @@
         <f t="shared" si="1"/>
         <v>4.9415500000000003</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="4">
         <f>VLOOKUP($F28,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1796,7 +1821,7 @@
         <f t="shared" si="1"/>
         <v>7.8376200000000003</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="4">
         <f>VLOOKUP($F29,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -1837,7 +1862,7 @@
         <f t="shared" si="1"/>
         <v>12.58432</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="4">
         <f>VLOOKUP($F30,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -1878,7 +1903,7 @@
         <f t="shared" si="1"/>
         <v>5.9415500000000003</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="4">
         <f>VLOOKUP($F31,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1919,7 +1944,7 @@
         <f t="shared" si="1"/>
         <v>8.4415499999999994</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="4">
         <f>VLOOKUP($F32,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -1960,7 +1985,7 @@
         <f t="shared" si="1"/>
         <v>3.4415499999999999</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="4">
         <f>VLOOKUP($F33,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2001,7 +2026,7 @@
         <f t="shared" si="1"/>
         <v>4.8376200000000003</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="4">
         <f>VLOOKUP($F34,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -2042,7 +2067,7 @@
         <f t="shared" si="1"/>
         <v>9.4415499999999994</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="4">
         <f>VLOOKUP($F35,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2083,7 +2108,7 @@
         <f t="shared" si="1"/>
         <v>7.4415500000000003</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="4">
         <f>VLOOKUP($F36,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2124,7 +2149,7 @@
         <f t="shared" si="1"/>
         <v>8.9415499999999994</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="4">
         <f>VLOOKUP($F37,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2165,7 +2190,7 @@
         <f t="shared" si="1"/>
         <v>7.9415500000000003</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="4">
         <f>VLOOKUP($F38,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2206,7 +2231,7 @@
         <f t="shared" si="1"/>
         <v>4.3376200000000003</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="4">
         <f>VLOOKUP($F39,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -2247,7 +2272,7 @@
         <f t="shared" si="1"/>
         <v>8.4415499999999994</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="4">
         <f>VLOOKUP($F40,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2288,7 +2313,7 @@
         <f t="shared" si="1"/>
         <v>8.4415499999999994</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="4">
         <f>VLOOKUP($F41,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2329,7 +2354,7 @@
         <f t="shared" si="1"/>
         <v>5.9415500000000003</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="4">
         <f>VLOOKUP($F42,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2370,7 +2395,7 @@
         <f t="shared" si="1"/>
         <v>9.9415499999999994</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="4">
         <f>VLOOKUP($F43,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2411,7 +2436,7 @@
         <f t="shared" si="1"/>
         <v>3.9415499999999999</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="4">
         <f>VLOOKUP($F44,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2452,7 +2477,7 @@
         <f t="shared" si="1"/>
         <v>6.4415500000000003</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="4">
         <f>VLOOKUP($F45,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2493,7 +2518,7 @@
         <f t="shared" si="1"/>
         <v>14.58432</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="4">
         <f>VLOOKUP($F46,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -2534,7 +2559,7 @@
         <f t="shared" si="1"/>
         <v>4.4415500000000003</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="4">
         <f>VLOOKUP($F47,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2575,7 +2600,7 @@
         <f t="shared" si="1"/>
         <v>6.9415500000000003</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48" s="4">
         <f>VLOOKUP($F48,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2616,7 +2641,7 @@
         <f t="shared" si="1"/>
         <v>10.941549999999999</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J49" s="4">
         <f>VLOOKUP($F49,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2657,7 +2682,7 @@
         <f t="shared" si="1"/>
         <v>14.941549999999999</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="4">
         <f>VLOOKUP($F50,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2698,7 +2723,7 @@
         <f t="shared" si="1"/>
         <v>10.941549999999999</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J51" s="4">
         <f>VLOOKUP($F51,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2739,7 +2764,7 @@
         <f t="shared" si="1"/>
         <v>4.9415500000000003</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J52" s="4">
         <f>VLOOKUP($F52,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2780,7 +2805,7 @@
         <f t="shared" si="1"/>
         <v>9.8376199999999994</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J53" s="4">
         <f>VLOOKUP($F53,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -2821,7 +2846,7 @@
         <f t="shared" si="1"/>
         <v>13.837619999999999</v>
       </c>
-      <c r="J54" s="2">
+      <c r="J54" s="4">
         <f>VLOOKUP($F54,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -2862,7 +2887,7 @@
         <f t="shared" si="1"/>
         <v>18.941549999999999</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="4">
         <f>VLOOKUP($F55,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2903,7 +2928,7 @@
         <f t="shared" si="1"/>
         <v>18.837620000000001</v>
       </c>
-      <c r="J56" s="2">
+      <c r="J56" s="4">
         <f>VLOOKUP($F56,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -2944,7 +2969,7 @@
         <f t="shared" si="1"/>
         <v>7.9415500000000003</v>
       </c>
-      <c r="J57" s="2">
+      <c r="J57" s="4">
         <f>VLOOKUP($F57,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -2985,7 +3010,7 @@
         <f t="shared" si="1"/>
         <v>2.8376199999999998</v>
       </c>
-      <c r="J58" s="2">
+      <c r="J58" s="4">
         <f>VLOOKUP($F58,sPathTypes!$A:$I,8,FALSE)</f>
         <v>7.3019999999999996</v>
       </c>
@@ -3026,7 +3051,7 @@
         <f t="shared" si="1"/>
         <v>7.9415500000000003</v>
       </c>
-      <c r="J59" s="2">
+      <c r="J59" s="4">
         <f>VLOOKUP($F59,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3067,7 +3092,7 @@
         <f t="shared" si="1"/>
         <v>6.9415500000000003</v>
       </c>
-      <c r="J60" s="2">
+      <c r="J60" s="4">
         <f>VLOOKUP($F60,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3108,7 +3133,7 @@
         <f t="shared" si="1"/>
         <v>7.4415500000000003</v>
       </c>
-      <c r="J61" s="2">
+      <c r="J61" s="4">
         <f>VLOOKUP($F61,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3149,7 +3174,7 @@
         <f t="shared" si="1"/>
         <v>9.4415499999999994</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="4">
         <f>VLOOKUP($F62,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3190,7 +3215,7 @@
         <f t="shared" si="1"/>
         <v>3.4415499999999999</v>
       </c>
-      <c r="J63" s="2">
+      <c r="J63" s="4">
         <f>VLOOKUP($F63,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3231,7 +3256,7 @@
         <f t="shared" si="1"/>
         <v>5.9415500000000003</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J64" s="4">
         <f>VLOOKUP($F64,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3272,7 +3297,7 @@
         <f t="shared" si="1"/>
         <v>8.4415499999999994</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="4">
         <f>VLOOKUP($F65,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3313,7 +3338,7 @@
         <f t="shared" si="1"/>
         <v>3.4415499999999999</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="4">
         <f>VLOOKUP($F66,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3339,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F78" si="2">IF(D67=30,"Secondary",IF(D67=50,"Main Type 1",IF(D67=80,"Main Type 2","Unknown")))</f>
+        <f t="shared" ref="F67:F81" si="2">IF(D67=30,"Secondary",IF(D67=50,"Main Type 1",IF(D67=80,"Main Type 2","Unknown")))</f>
         <v>Secondary</v>
       </c>
       <c r="G67">
@@ -3351,10 +3376,10 @@
         <v>5.8450000000000002E-2</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I78" si="3">C67-H67</f>
+        <f t="shared" ref="I67:I81" si="3">C67-H67</f>
         <v>8.4415499999999994</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="4">
         <f>VLOOKUP($F67,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3395,7 +3420,7 @@
         <f t="shared" si="3"/>
         <v>9.58432</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68" s="4">
         <f>VLOOKUP($F68,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -3436,7 +3461,7 @@
         <f t="shared" si="3"/>
         <v>2.3415499999999998</v>
       </c>
-      <c r="J69" s="2">
+      <c r="J69" s="4">
         <f>VLOOKUP($F69,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3477,7 +3502,7 @@
         <f t="shared" si="3"/>
         <v>3.4415499999999999</v>
       </c>
-      <c r="J70" s="2">
+      <c r="J70" s="4">
         <f>VLOOKUP($F70,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3518,7 +3543,7 @@
         <f t="shared" si="3"/>
         <v>3.4415499999999999</v>
       </c>
-      <c r="J71" s="2">
+      <c r="J71" s="4">
         <f>VLOOKUP($F71,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3559,7 +3584,7 @@
         <f t="shared" si="3"/>
         <v>7.4415500000000003</v>
       </c>
-      <c r="J72" s="2">
+      <c r="J72" s="4">
         <f>VLOOKUP($F72,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3600,7 +3625,7 @@
         <f t="shared" si="3"/>
         <v>4.4415500000000003</v>
       </c>
-      <c r="J73" s="2">
+      <c r="J73" s="4">
         <f>VLOOKUP($F73,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3641,7 +3666,7 @@
         <f t="shared" si="3"/>
         <v>6.4415500000000003</v>
       </c>
-      <c r="J74" s="2">
+      <c r="J74" s="4">
         <f>VLOOKUP($F74,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3682,7 +3707,7 @@
         <f t="shared" si="3"/>
         <v>8.4415499999999994</v>
       </c>
-      <c r="J75" s="2">
+      <c r="J75" s="4">
         <f>VLOOKUP($F75,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3723,7 +3748,7 @@
         <f t="shared" si="3"/>
         <v>7.58432</v>
       </c>
-      <c r="J76" s="2">
+      <c r="J76" s="4">
         <f>VLOOKUP($F76,sPathTypes!$A:$I,8,FALSE)</f>
         <v>15.19</v>
       </c>
@@ -3764,7 +3789,7 @@
         <f t="shared" si="3"/>
         <v>6.4415500000000003</v>
       </c>
-      <c r="J77" s="2">
+      <c r="J77" s="4">
         <f>VLOOKUP($F77,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3805,7 +3830,7 @@
         <f t="shared" si="3"/>
         <v>6.9415500000000003</v>
       </c>
-      <c r="J78" s="2">
+      <c r="J78" s="4">
         <f>VLOOKUP($F78,sPathTypes!$A:$I,8,FALSE)</f>
         <v>4.444</v>
       </c>
@@ -3814,7 +3839,201 @@
         <v>2.24E-2</v>
       </c>
     </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="5">
+        <v>38</v>
+      </c>
+      <c r="B79" s="5">
+        <v>20</v>
+      </c>
+      <c r="C79" s="6">
+        <v>11</v>
+      </c>
+      <c r="D79" s="6">
+        <v>30</v>
+      </c>
+      <c r="E79" s="6">
+        <v>0</v>
+      </c>
+      <c r="F79" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G79" s="6">
+        <f>VLOOKUP($F79,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H79" s="6">
+        <f>VLOOKUP($F79,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I79" s="6">
+        <f t="shared" si="3"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J79" s="6">
+        <f>VLOOKUP($F79,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K79" s="6">
+        <f>VLOOKUP($F79,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="5">
+        <v>38</v>
+      </c>
+      <c r="B80" s="5">
+        <v>22</v>
+      </c>
+      <c r="C80" s="6">
+        <v>15</v>
+      </c>
+      <c r="D80" s="6">
+        <v>30</v>
+      </c>
+      <c r="E80" s="6">
+        <v>0</v>
+      </c>
+      <c r="F80" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G80" s="6">
+        <f>VLOOKUP($F80,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H80" s="6">
+        <f>VLOOKUP($F80,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I80" s="6">
+        <f t="shared" si="3"/>
+        <v>14.941549999999999</v>
+      </c>
+      <c r="J80" s="6">
+        <f>VLOOKUP($F80,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K80" s="6">
+        <f>VLOOKUP($F80,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>38</v>
+      </c>
+      <c r="B81" s="5">
+        <v>26</v>
+      </c>
+      <c r="C81" s="6">
+        <v>11</v>
+      </c>
+      <c r="D81" s="6">
+        <v>30</v>
+      </c>
+      <c r="E81" s="6">
+        <v>0</v>
+      </c>
+      <c r="F81" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G81" s="6">
+        <f>VLOOKUP($F81,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H81" s="6">
+        <f>VLOOKUP($F81,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I81" s="6">
+        <f t="shared" si="3"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J81" s="6">
+        <f>VLOOKUP($F81,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K81" s="6">
+        <f>VLOOKUP($F81,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>23</v>
+      </c>
+      <c r="B82" s="5">
+        <v>38</v>
+      </c>
+      <c r="C82" s="6">
+        <v>7</v>
+      </c>
+      <c r="D82" s="6">
+        <v>30</v>
+      </c>
+      <c r="E82" s="6">
+        <v>0</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G82" s="6">
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H82" s="6">
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I82" s="6">
+        <v>6.9415500000000003</v>
+      </c>
+      <c r="J82" s="6">
+        <v>4.444</v>
+      </c>
+      <c r="K82" s="6">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
+        <v>25</v>
+      </c>
+      <c r="B83" s="5">
+        <v>38</v>
+      </c>
+      <c r="C83" s="6">
+        <v>5</v>
+      </c>
+      <c r="D83" s="6">
+        <v>30</v>
+      </c>
+      <c r="E83" s="6">
+        <v>0</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="6">
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H83" s="6">
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I83" s="6">
+        <v>4.9415500000000003</v>
+      </c>
+      <c r="J83" s="6">
+        <v>4.444</v>
+      </c>
+      <c r="K83" s="6">
+        <v>2.24E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:K83" xr:uid="{3C34D7CB-5337-4A22-B32E-222A13B8F8D6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3836,7 +4055,7 @@
     <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3862,7 +4081,7 @@
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3893,7 +4112,7 @@
         <f>(B2+D2)/1000</f>
         <v>5.8450000000000002E-2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>4.444</v>
       </c>
       <c r="I2">
@@ -3924,7 +4143,7 @@
         <f t="shared" ref="G3:G4" si="0">(B3+D3)/1000</f>
         <v>0.16238</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>7.3019999999999996</v>
       </c>
       <c r="I3">
@@ -3955,7 +4174,7 @@
         <f t="shared" si="0"/>
         <v>0.41567999999999999</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>15.19</v>
       </c>
       <c r="I4">
@@ -3971,13 +4190,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" style="5" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -3985,7 +4204,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4002,7 +4221,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -4019,7 +4238,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -4036,41 +4255,41 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>0.25</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>24</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>0.25</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>24</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
       <c r="B6" s="1">
@@ -4087,24 +4306,24 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>17</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>0.25</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>1</v>
       </c>
       <c r="B8" s="1">
@@ -4121,7 +4340,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9" s="5">
         <v>2</v>
       </c>
       <c r="B9" s="1">
@@ -4138,42 +4357,42 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>23</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>0.25</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>25</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>0.25</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>24</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>0</v>
       </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>2</v>
       </c>
       <c r="B12" s="1">
@@ -4190,7 +4409,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>3</v>
       </c>
       <c r="B13" s="1">
@@ -4207,24 +4426,24 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>30</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="5">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6">
         <v>0.25</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>24</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="A15" s="5">
         <v>2</v>
       </c>
       <c r="B15" s="1">
@@ -4260,8 +4479,8 @@
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4278,10 +4497,10 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4298,10 +4517,10 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>0.25</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>0.96</v>
       </c>
     </row>
@@ -4318,10 +4537,10 @@
       <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>0.25</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>0.96</v>
       </c>
     </row>
@@ -4338,10 +4557,10 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>0.25</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>0.96</v>
       </c>
     </row>
@@ -4358,10 +4577,10 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>0.25</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>0.96</v>
       </c>
     </row>
@@ -4378,10 +4597,10 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>0.25</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>0.96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solve model and save solution
</commit_message>
<xml_diff>
--- a/data/37-intersection map.xlsx
+++ b/data/37-intersection map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80edabada1d31728/FolderSync/University/TFM EV Routing/A Routing Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Documents\GitHub\TFM-EV-Routing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="11_F25DC773A252ABDACC10480D99185B725ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFD3368F-712B-478B-9A6C-9EF0F0E689B5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2F9A6E-3895-4BC7-B894-96B3E7243EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unindexed" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>pDelayPenalty [$/h]</t>
   </si>
@@ -170,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +214,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,6 +258,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,10 +275,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597D70E4-2172-494A-AB5D-BB966B7F274D}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -625,10 +638,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C34D7CB-5337-4A22-B32E-222A13B8F8D6}">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4029,6 +4042,3356 @@
         <v>4.444</v>
       </c>
       <c r="K83" s="6">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="7">
+        <v>8</v>
+      </c>
+      <c r="B84" s="7">
+        <v>1</v>
+      </c>
+      <c r="C84" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D84" s="8">
+        <v>50</v>
+      </c>
+      <c r="E84" s="8">
+        <v>0</v>
+      </c>
+      <c r="F84" s="8" t="str">
+        <f>IF(D84=30,"Secondary",IF(D84=50,"Main Type 1",IF(D84=80,"Main Type 2","Unknown")))</f>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G84" s="8">
+        <f>VLOOKUP($F84,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H84" s="8">
+        <f>VLOOKUP($F84,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I84" s="8">
+        <f>C84-H84</f>
+        <v>7.3376200000000003</v>
+      </c>
+      <c r="J84" s="8">
+        <f>VLOOKUP($F84,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K84" s="8">
+        <f>VLOOKUP($F84,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="7">
+        <v>10</v>
+      </c>
+      <c r="B85" s="7">
+        <v>1</v>
+      </c>
+      <c r="C85" s="8">
+        <v>10</v>
+      </c>
+      <c r="D85" s="8">
+        <v>50</v>
+      </c>
+      <c r="E85" s="8">
+        <v>0</v>
+      </c>
+      <c r="F85" s="8" t="str">
+        <f t="shared" ref="F85:F148" si="4">IF(D85=30,"Secondary",IF(D85=50,"Main Type 1",IF(D85=80,"Main Type 2","Unknown")))</f>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G85" s="8">
+        <f>VLOOKUP($F85,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H85" s="8">
+        <f>VLOOKUP($F85,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I85" s="8">
+        <f t="shared" ref="I85:I148" si="5">C85-H85</f>
+        <v>9.8376199999999994</v>
+      </c>
+      <c r="J85" s="8">
+        <f>VLOOKUP($F85,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K85" s="8">
+        <f>VLOOKUP($F85,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="7">
+        <v>1</v>
+      </c>
+      <c r="B86" s="7">
+        <v>2</v>
+      </c>
+      <c r="C86" s="8">
+        <v>11</v>
+      </c>
+      <c r="D86" s="8">
+        <v>30</v>
+      </c>
+      <c r="E86" s="8">
+        <v>0</v>
+      </c>
+      <c r="F86" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G86" s="8">
+        <f>VLOOKUP($F86,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H86" s="8">
+        <f>VLOOKUP($F86,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I86" s="8">
+        <f t="shared" si="5"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J86" s="8">
+        <f>VLOOKUP($F86,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K86" s="8">
+        <f>VLOOKUP($F86,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="7">
+        <v>5</v>
+      </c>
+      <c r="B87" s="7">
+        <v>2</v>
+      </c>
+      <c r="C87" s="8">
+        <v>10</v>
+      </c>
+      <c r="D87" s="8">
+        <v>30</v>
+      </c>
+      <c r="E87" s="8">
+        <v>0</v>
+      </c>
+      <c r="F87" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G87" s="8">
+        <f>VLOOKUP($F87,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H87" s="8">
+        <f>VLOOKUP($F87,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I87" s="8">
+        <f t="shared" si="5"/>
+        <v>9.9415499999999994</v>
+      </c>
+      <c r="J87" s="8">
+        <f>VLOOKUP($F87,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K87" s="8">
+        <f>VLOOKUP($F87,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="7">
+        <v>7</v>
+      </c>
+      <c r="B88" s="7">
+        <v>2</v>
+      </c>
+      <c r="C88" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="D88" s="8">
+        <v>30</v>
+      </c>
+      <c r="E88" s="8">
+        <v>0</v>
+      </c>
+      <c r="F88" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G88" s="8">
+        <f>VLOOKUP($F88,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H88" s="8">
+        <f>VLOOKUP($F88,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I88" s="8">
+        <f t="shared" si="5"/>
+        <v>1.1415500000000001</v>
+      </c>
+      <c r="J88" s="8">
+        <f>VLOOKUP($F88,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K88" s="8">
+        <f>VLOOKUP($F88,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7">
+        <v>2</v>
+      </c>
+      <c r="B89" s="7">
+        <v>3</v>
+      </c>
+      <c r="C89" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="D89" s="8">
+        <v>30</v>
+      </c>
+      <c r="E89" s="8">
+        <v>0</v>
+      </c>
+      <c r="F89" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G89" s="8">
+        <f>VLOOKUP($F89,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H89" s="8">
+        <f>VLOOKUP($F89,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I89" s="8">
+        <f t="shared" si="5"/>
+        <v>6.4415500000000003</v>
+      </c>
+      <c r="J89" s="8">
+        <f>VLOOKUP($F89,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K89" s="8">
+        <f>VLOOKUP($F89,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="7">
+        <v>3</v>
+      </c>
+      <c r="B90" s="7">
+        <v>4</v>
+      </c>
+      <c r="C90" s="8">
+        <v>3</v>
+      </c>
+      <c r="D90" s="8">
+        <v>30</v>
+      </c>
+      <c r="E90" s="8">
+        <v>0</v>
+      </c>
+      <c r="F90" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G90" s="8">
+        <f>VLOOKUP($F90,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H90" s="8">
+        <f>VLOOKUP($F90,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I90" s="8">
+        <f t="shared" si="5"/>
+        <v>2.9415499999999999</v>
+      </c>
+      <c r="J90" s="8">
+        <f>VLOOKUP($F90,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K90" s="8">
+        <f>VLOOKUP($F90,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="7">
+        <v>5</v>
+      </c>
+      <c r="B91" s="7">
+        <v>4</v>
+      </c>
+      <c r="C91" s="8">
+        <v>5</v>
+      </c>
+      <c r="D91" s="8">
+        <v>80</v>
+      </c>
+      <c r="E91" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F91" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G91" s="8">
+        <f>VLOOKUP($F91,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H91" s="8">
+        <f>VLOOKUP($F91,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I91" s="8">
+        <f t="shared" si="5"/>
+        <v>4.58432</v>
+      </c>
+      <c r="J91" s="8">
+        <f>VLOOKUP($F91,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K91" s="8">
+        <f>VLOOKUP($F91,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="7">
+        <v>3</v>
+      </c>
+      <c r="B92" s="7">
+        <v>5</v>
+      </c>
+      <c r="C92" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="D92" s="8">
+        <v>30</v>
+      </c>
+      <c r="E92" s="8">
+        <v>0</v>
+      </c>
+      <c r="F92" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G92" s="8">
+        <f>VLOOKUP($F92,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H92" s="8">
+        <f>VLOOKUP($F92,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I92" s="8">
+        <f t="shared" si="5"/>
+        <v>6.4415500000000003</v>
+      </c>
+      <c r="J92" s="8">
+        <f>VLOOKUP($F92,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K92" s="8">
+        <f>VLOOKUP($F92,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="7">
+        <v>8</v>
+      </c>
+      <c r="B93" s="7">
+        <v>5</v>
+      </c>
+      <c r="C93" s="8">
+        <v>12</v>
+      </c>
+      <c r="D93" s="8">
+        <v>50</v>
+      </c>
+      <c r="E93" s="8">
+        <v>0</v>
+      </c>
+      <c r="F93" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G93" s="8">
+        <f>VLOOKUP($F93,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H93" s="8">
+        <f>VLOOKUP($F93,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I93" s="8">
+        <f t="shared" si="5"/>
+        <v>11.837619999999999</v>
+      </c>
+      <c r="J93" s="8">
+        <f>VLOOKUP($F93,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K93" s="8">
+        <f>VLOOKUP($F93,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="7">
+        <v>14</v>
+      </c>
+      <c r="B94" s="7">
+        <v>5</v>
+      </c>
+      <c r="C94" s="8">
+        <v>6</v>
+      </c>
+      <c r="D94" s="8">
+        <v>80</v>
+      </c>
+      <c r="E94" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F94" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G94" s="8">
+        <f>VLOOKUP($F94,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H94" s="8">
+        <f>VLOOKUP($F94,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I94" s="8">
+        <f t="shared" si="5"/>
+        <v>5.58432</v>
+      </c>
+      <c r="J94" s="8">
+        <f>VLOOKUP($F94,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K94" s="8">
+        <f>VLOOKUP($F94,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="7">
+        <v>12</v>
+      </c>
+      <c r="B95" s="7">
+        <v>6</v>
+      </c>
+      <c r="C95" s="8">
+        <v>4</v>
+      </c>
+      <c r="D95" s="8">
+        <v>30</v>
+      </c>
+      <c r="E95" s="8">
+        <v>0</v>
+      </c>
+      <c r="F95" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G95" s="8">
+        <f>VLOOKUP($F95,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H95" s="8">
+        <f>VLOOKUP($F95,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I95" s="8">
+        <f t="shared" si="5"/>
+        <v>3.9415499999999999</v>
+      </c>
+      <c r="J95" s="8">
+        <f>VLOOKUP($F95,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K95" s="8">
+        <f>VLOOKUP($F95,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="7">
+        <v>13</v>
+      </c>
+      <c r="B96" s="7">
+        <v>6</v>
+      </c>
+      <c r="C96" s="8">
+        <v>4</v>
+      </c>
+      <c r="D96" s="8">
+        <v>30</v>
+      </c>
+      <c r="E96" s="8">
+        <v>0</v>
+      </c>
+      <c r="F96" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G96" s="8">
+        <f>VLOOKUP($F96,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H96" s="8">
+        <f>VLOOKUP($F96,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I96" s="8">
+        <f t="shared" si="5"/>
+        <v>3.9415499999999999</v>
+      </c>
+      <c r="J96" s="8">
+        <f>VLOOKUP($F96,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K96" s="8">
+        <f>VLOOKUP($F96,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="7">
+        <v>1</v>
+      </c>
+      <c r="B97" s="7">
+        <v>7</v>
+      </c>
+      <c r="C97" s="8">
+        <v>8</v>
+      </c>
+      <c r="D97" s="8">
+        <v>30</v>
+      </c>
+      <c r="E97" s="8">
+        <v>0</v>
+      </c>
+      <c r="F97" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G97" s="8">
+        <f>VLOOKUP($F97,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H97" s="8">
+        <f>VLOOKUP($F97,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I97" s="8">
+        <f t="shared" si="5"/>
+        <v>7.9415500000000003</v>
+      </c>
+      <c r="J97" s="8">
+        <f>VLOOKUP($F97,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K97" s="8">
+        <f>VLOOKUP($F97,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="7">
+        <v>8</v>
+      </c>
+      <c r="B98" s="7">
+        <v>7</v>
+      </c>
+      <c r="C98" s="8">
+        <v>9.5</v>
+      </c>
+      <c r="D98" s="8">
+        <v>30</v>
+      </c>
+      <c r="E98" s="8">
+        <v>0</v>
+      </c>
+      <c r="F98" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G98" s="8">
+        <f>VLOOKUP($F98,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H98" s="8">
+        <f>VLOOKUP($F98,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I98" s="8">
+        <f t="shared" si="5"/>
+        <v>9.4415499999999994</v>
+      </c>
+      <c r="J98" s="8">
+        <f>VLOOKUP($F98,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K98" s="8">
+        <f>VLOOKUP($F98,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="7">
+        <v>6</v>
+      </c>
+      <c r="B99" s="7">
+        <v>8</v>
+      </c>
+      <c r="C99" s="8">
+        <v>5</v>
+      </c>
+      <c r="D99" s="8">
+        <v>30</v>
+      </c>
+      <c r="E99" s="8">
+        <v>0</v>
+      </c>
+      <c r="F99" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G99" s="8">
+        <f>VLOOKUP($F99,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H99" s="8">
+        <f>VLOOKUP($F99,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I99" s="8">
+        <f t="shared" si="5"/>
+        <v>4.9415500000000003</v>
+      </c>
+      <c r="J99" s="8">
+        <f>VLOOKUP($F99,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K99" s="8">
+        <f>VLOOKUP($F99,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="7">
+        <v>9</v>
+      </c>
+      <c r="B100" s="7">
+        <v>8</v>
+      </c>
+      <c r="C100" s="8">
+        <v>15</v>
+      </c>
+      <c r="D100" s="8">
+        <v>30</v>
+      </c>
+      <c r="E100" s="8">
+        <v>0</v>
+      </c>
+      <c r="F100" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G100" s="8">
+        <f>VLOOKUP($F100,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H100" s="8">
+        <f>VLOOKUP($F100,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I100" s="8">
+        <f t="shared" si="5"/>
+        <v>14.941549999999999</v>
+      </c>
+      <c r="J100" s="8">
+        <f>VLOOKUP($F100,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K100" s="8">
+        <f>VLOOKUP($F100,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="7">
+        <v>15</v>
+      </c>
+      <c r="B101" s="7">
+        <v>8</v>
+      </c>
+      <c r="C101" s="8">
+        <v>13</v>
+      </c>
+      <c r="D101" s="8">
+        <v>30</v>
+      </c>
+      <c r="E101" s="8">
+        <v>0</v>
+      </c>
+      <c r="F101" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G101" s="8">
+        <f>VLOOKUP($F101,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H101" s="8">
+        <f>VLOOKUP($F101,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I101" s="8">
+        <f t="shared" si="5"/>
+        <v>12.941549999999999</v>
+      </c>
+      <c r="J101" s="8">
+        <f>VLOOKUP($F101,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K101" s="8">
+        <f>VLOOKUP($F101,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="7">
+        <v>15</v>
+      </c>
+      <c r="B102" s="7">
+        <v>9</v>
+      </c>
+      <c r="C102" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D102" s="8">
+        <v>30</v>
+      </c>
+      <c r="E102" s="8">
+        <v>0</v>
+      </c>
+      <c r="F102" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G102" s="8">
+        <f>VLOOKUP($F102,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H102" s="8">
+        <f>VLOOKUP($F102,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I102" s="8">
+        <f t="shared" si="5"/>
+        <v>3.4415499999999999</v>
+      </c>
+      <c r="J102" s="8">
+        <f>VLOOKUP($F102,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K102" s="8">
+        <f>VLOOKUP($F102,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="7">
+        <v>19</v>
+      </c>
+      <c r="B103" s="7">
+        <v>9</v>
+      </c>
+      <c r="C103" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D103" s="8">
+        <v>30</v>
+      </c>
+      <c r="E103" s="8">
+        <v>0</v>
+      </c>
+      <c r="F103" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G103" s="8">
+        <f>VLOOKUP($F103,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H103" s="8">
+        <f>VLOOKUP($F103,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I103" s="8">
+        <f t="shared" si="5"/>
+        <v>7.4415500000000003</v>
+      </c>
+      <c r="J103" s="8">
+        <f>VLOOKUP($F103,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K103" s="8">
+        <f>VLOOKUP($F103,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="7">
+        <v>11</v>
+      </c>
+      <c r="B104" s="7">
+        <v>10</v>
+      </c>
+      <c r="C104" s="8">
+        <v>5</v>
+      </c>
+      <c r="D104" s="8">
+        <v>50</v>
+      </c>
+      <c r="E104" s="8">
+        <v>0</v>
+      </c>
+      <c r="F104" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G104" s="8">
+        <f>VLOOKUP($F104,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H104" s="8">
+        <f>VLOOKUP($F104,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I104" s="8">
+        <f t="shared" si="5"/>
+        <v>4.8376200000000003</v>
+      </c>
+      <c r="J104" s="8">
+        <f>VLOOKUP($F104,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K104" s="8">
+        <f>VLOOKUP($F104,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="7">
+        <v>19</v>
+      </c>
+      <c r="B105" s="7">
+        <v>11</v>
+      </c>
+      <c r="C105" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="D105" s="8">
+        <v>30</v>
+      </c>
+      <c r="E105" s="8">
+        <v>0</v>
+      </c>
+      <c r="F105" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G105" s="8">
+        <f>VLOOKUP($F105,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H105" s="8">
+        <f>VLOOKUP($F105,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I105" s="8">
+        <f t="shared" si="5"/>
+        <v>6.4415500000000003</v>
+      </c>
+      <c r="J105" s="8">
+        <f>VLOOKUP($F105,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K105" s="8">
+        <f>VLOOKUP($F105,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="7">
+        <v>22</v>
+      </c>
+      <c r="B106" s="7">
+        <v>11</v>
+      </c>
+      <c r="C106" s="8">
+        <v>14</v>
+      </c>
+      <c r="D106" s="8">
+        <v>80</v>
+      </c>
+      <c r="E106" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F106" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G106" s="8">
+        <f>VLOOKUP($F106,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H106" s="8">
+        <f>VLOOKUP($F106,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I106" s="8">
+        <f t="shared" si="5"/>
+        <v>13.58432</v>
+      </c>
+      <c r="J106" s="8">
+        <f>VLOOKUP($F106,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K106" s="8">
+        <f>VLOOKUP($F106,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="7">
+        <v>13</v>
+      </c>
+      <c r="B107" s="7">
+        <v>12</v>
+      </c>
+      <c r="C107" s="8">
+        <v>6</v>
+      </c>
+      <c r="D107" s="8">
+        <v>30</v>
+      </c>
+      <c r="E107" s="8">
+        <v>0</v>
+      </c>
+      <c r="F107" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G107" s="8">
+        <f>VLOOKUP($F107,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H107" s="8">
+        <f>VLOOKUP($F107,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I107" s="8">
+        <f t="shared" si="5"/>
+        <v>5.9415500000000003</v>
+      </c>
+      <c r="J107" s="8">
+        <f>VLOOKUP($F107,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K107" s="8">
+        <f>VLOOKUP($F107,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="7">
+        <v>16</v>
+      </c>
+      <c r="B108" s="7">
+        <v>12</v>
+      </c>
+      <c r="C108" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D108" s="8">
+        <v>30</v>
+      </c>
+      <c r="E108" s="8">
+        <v>0</v>
+      </c>
+      <c r="F108" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G108" s="8">
+        <f>VLOOKUP($F108,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H108" s="8">
+        <f>VLOOKUP($F108,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I108" s="8">
+        <f t="shared" si="5"/>
+        <v>7.4415500000000003</v>
+      </c>
+      <c r="J108" s="8">
+        <f>VLOOKUP($F108,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K108" s="8">
+        <f>VLOOKUP($F108,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="7">
+        <v>5</v>
+      </c>
+      <c r="B109" s="7">
+        <v>13</v>
+      </c>
+      <c r="C109" s="8">
+        <v>6</v>
+      </c>
+      <c r="D109" s="8">
+        <v>30</v>
+      </c>
+      <c r="E109" s="8">
+        <v>0</v>
+      </c>
+      <c r="F109" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G109" s="8">
+        <f>VLOOKUP($F109,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H109" s="8">
+        <f>VLOOKUP($F109,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I109" s="8">
+        <f t="shared" si="5"/>
+        <v>5.9415500000000003</v>
+      </c>
+      <c r="J109" s="8">
+        <f>VLOOKUP($F109,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K109" s="8">
+        <f>VLOOKUP($F109,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="7">
+        <v>13</v>
+      </c>
+      <c r="B110" s="7">
+        <v>14</v>
+      </c>
+      <c r="C110" s="8">
+        <v>5</v>
+      </c>
+      <c r="D110" s="8">
+        <v>30</v>
+      </c>
+      <c r="E110" s="8">
+        <v>0</v>
+      </c>
+      <c r="F110" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G110" s="8">
+        <f>VLOOKUP($F110,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H110" s="8">
+        <f>VLOOKUP($F110,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I110" s="8">
+        <f t="shared" si="5"/>
+        <v>4.9415500000000003</v>
+      </c>
+      <c r="J110" s="8">
+        <f>VLOOKUP($F110,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K110" s="8">
+        <f>VLOOKUP($F110,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="7">
+        <v>16</v>
+      </c>
+      <c r="B111" s="7">
+        <v>14</v>
+      </c>
+      <c r="C111" s="8">
+        <v>8</v>
+      </c>
+      <c r="D111" s="8">
+        <v>50</v>
+      </c>
+      <c r="E111" s="8">
+        <v>0</v>
+      </c>
+      <c r="F111" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G111" s="8">
+        <f>VLOOKUP($F111,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H111" s="8">
+        <f>VLOOKUP($F111,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I111" s="8">
+        <f t="shared" si="5"/>
+        <v>7.8376200000000003</v>
+      </c>
+      <c r="J111" s="8">
+        <f>VLOOKUP($F111,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K111" s="8">
+        <f>VLOOKUP($F111,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="7">
+        <v>31</v>
+      </c>
+      <c r="B112" s="7">
+        <v>14</v>
+      </c>
+      <c r="C112" s="8">
+        <v>13</v>
+      </c>
+      <c r="D112" s="8">
+        <v>80</v>
+      </c>
+      <c r="E112" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F112" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G112" s="8">
+        <f>VLOOKUP($F112,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H112" s="8">
+        <f>VLOOKUP($F112,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I112" s="8">
+        <f t="shared" si="5"/>
+        <v>12.58432</v>
+      </c>
+      <c r="J112" s="8">
+        <f>VLOOKUP($F112,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K112" s="8">
+        <f>VLOOKUP($F112,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="7">
+        <v>16</v>
+      </c>
+      <c r="B113" s="7">
+        <v>15</v>
+      </c>
+      <c r="C113" s="8">
+        <v>6</v>
+      </c>
+      <c r="D113" s="8">
+        <v>30</v>
+      </c>
+      <c r="E113" s="8">
+        <v>0</v>
+      </c>
+      <c r="F113" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G113" s="8">
+        <f>VLOOKUP($F113,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H113" s="8">
+        <f>VLOOKUP($F113,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I113" s="8">
+        <f t="shared" si="5"/>
+        <v>5.9415500000000003</v>
+      </c>
+      <c r="J113" s="8">
+        <f>VLOOKUP($F113,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K113" s="8">
+        <f>VLOOKUP($F113,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="7">
+        <v>8</v>
+      </c>
+      <c r="B114" s="7">
+        <v>16</v>
+      </c>
+      <c r="C114" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D114" s="8">
+        <v>30</v>
+      </c>
+      <c r="E114" s="8">
+        <v>0</v>
+      </c>
+      <c r="F114" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G114" s="8">
+        <f>VLOOKUP($F114,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H114" s="8">
+        <f>VLOOKUP($F114,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I114" s="8">
+        <f t="shared" si="5"/>
+        <v>8.4415499999999994</v>
+      </c>
+      <c r="J114" s="8">
+        <f>VLOOKUP($F114,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K114" s="8">
+        <f>VLOOKUP($F114,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="7">
+        <v>17</v>
+      </c>
+      <c r="B115" s="7">
+        <v>16</v>
+      </c>
+      <c r="C115" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D115" s="8">
+        <v>30</v>
+      </c>
+      <c r="E115" s="8">
+        <v>0</v>
+      </c>
+      <c r="F115" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G115" s="8">
+        <f>VLOOKUP($F115,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H115" s="8">
+        <f>VLOOKUP($F115,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I115" s="8">
+        <f t="shared" si="5"/>
+        <v>3.4415499999999999</v>
+      </c>
+      <c r="J115" s="8">
+        <f>VLOOKUP($F115,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K115" s="8">
+        <f>VLOOKUP($F115,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="7">
+        <v>18</v>
+      </c>
+      <c r="B116" s="7">
+        <v>16</v>
+      </c>
+      <c r="C116" s="8">
+        <v>5</v>
+      </c>
+      <c r="D116" s="8">
+        <v>50</v>
+      </c>
+      <c r="E116" s="8">
+        <v>0</v>
+      </c>
+      <c r="F116" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G116" s="8">
+        <f>VLOOKUP($F116,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H116" s="8">
+        <f>VLOOKUP($F116,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I116" s="8">
+        <f t="shared" si="5"/>
+        <v>4.8376200000000003</v>
+      </c>
+      <c r="J116" s="8">
+        <f>VLOOKUP($F116,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K116" s="8">
+        <f>VLOOKUP($F116,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="7">
+        <v>19</v>
+      </c>
+      <c r="B117" s="7">
+        <v>16</v>
+      </c>
+      <c r="C117" s="8">
+        <v>9.5</v>
+      </c>
+      <c r="D117" s="8">
+        <v>30</v>
+      </c>
+      <c r="E117" s="8">
+        <v>0</v>
+      </c>
+      <c r="F117" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G117" s="8">
+        <f>VLOOKUP($F117,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H117" s="8">
+        <f>VLOOKUP($F117,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I117" s="8">
+        <f t="shared" si="5"/>
+        <v>9.4415499999999994</v>
+      </c>
+      <c r="J117" s="8">
+        <f>VLOOKUP($F117,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K117" s="8">
+        <f>VLOOKUP($F117,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="7">
+        <v>18</v>
+      </c>
+      <c r="B118" s="7">
+        <v>17</v>
+      </c>
+      <c r="C118" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D118" s="8">
+        <v>30</v>
+      </c>
+      <c r="E118" s="8">
+        <v>0</v>
+      </c>
+      <c r="F118" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G118" s="8">
+        <f>VLOOKUP($F118,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H118" s="8">
+        <f>VLOOKUP($F118,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I118" s="8">
+        <f t="shared" si="5"/>
+        <v>7.4415500000000003</v>
+      </c>
+      <c r="J118" s="8">
+        <f>VLOOKUP($F118,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K118" s="8">
+        <f>VLOOKUP($F118,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="7">
+        <v>31</v>
+      </c>
+      <c r="B119" s="7">
+        <v>17</v>
+      </c>
+      <c r="C119" s="8">
+        <v>9</v>
+      </c>
+      <c r="D119" s="8">
+        <v>30</v>
+      </c>
+      <c r="E119" s="8">
+        <v>0</v>
+      </c>
+      <c r="F119" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G119" s="8">
+        <f>VLOOKUP($F119,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H119" s="8">
+        <f>VLOOKUP($F119,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I119" s="8">
+        <f t="shared" si="5"/>
+        <v>8.9415499999999994</v>
+      </c>
+      <c r="J119" s="8">
+        <f>VLOOKUP($F119,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K119" s="8">
+        <f>VLOOKUP($F119,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="7">
+        <v>27</v>
+      </c>
+      <c r="B120" s="7">
+        <v>18</v>
+      </c>
+      <c r="C120" s="8">
+        <v>8</v>
+      </c>
+      <c r="D120" s="8">
+        <v>30</v>
+      </c>
+      <c r="E120" s="8">
+        <v>0</v>
+      </c>
+      <c r="F120" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G120" s="8">
+        <f>VLOOKUP($F120,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H120" s="8">
+        <f>VLOOKUP($F120,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I120" s="8">
+        <f t="shared" si="5"/>
+        <v>7.9415500000000003</v>
+      </c>
+      <c r="J120" s="8">
+        <f>VLOOKUP($F120,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K120" s="8">
+        <f>VLOOKUP($F120,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="7">
+        <v>28</v>
+      </c>
+      <c r="B121" s="7">
+        <v>18</v>
+      </c>
+      <c r="C121" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="D121" s="8">
+        <v>50</v>
+      </c>
+      <c r="E121" s="8">
+        <v>0</v>
+      </c>
+      <c r="F121" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G121" s="8">
+        <f>VLOOKUP($F121,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H121" s="8">
+        <f>VLOOKUP($F121,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I121" s="8">
+        <f t="shared" si="5"/>
+        <v>4.3376200000000003</v>
+      </c>
+      <c r="J121" s="8">
+        <f>VLOOKUP($F121,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K121" s="8">
+        <f>VLOOKUP($F121,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="7">
+        <v>29</v>
+      </c>
+      <c r="B122" s="7">
+        <v>18</v>
+      </c>
+      <c r="C122" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D122" s="8">
+        <v>30</v>
+      </c>
+      <c r="E122" s="8">
+        <v>0</v>
+      </c>
+      <c r="F122" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G122" s="8">
+        <f>VLOOKUP($F122,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H122" s="8">
+        <f>VLOOKUP($F122,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I122" s="8">
+        <f t="shared" si="5"/>
+        <v>8.4415499999999994</v>
+      </c>
+      <c r="J122" s="8">
+        <f>VLOOKUP($F122,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K122" s="8">
+        <f>VLOOKUP($F122,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="7">
+        <v>20</v>
+      </c>
+      <c r="B123" s="7">
+        <v>19</v>
+      </c>
+      <c r="C123" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D123" s="8">
+        <v>30</v>
+      </c>
+      <c r="E123" s="8">
+        <v>0</v>
+      </c>
+      <c r="F123" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G123" s="8">
+        <f>VLOOKUP($F123,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H123" s="8">
+        <f>VLOOKUP($F123,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I123" s="8">
+        <f t="shared" si="5"/>
+        <v>8.4415499999999994</v>
+      </c>
+      <c r="J123" s="8">
+        <f>VLOOKUP($F123,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K123" s="8">
+        <f>VLOOKUP($F123,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="7">
+        <v>21</v>
+      </c>
+      <c r="B124" s="7">
+        <v>19</v>
+      </c>
+      <c r="C124" s="8">
+        <v>6</v>
+      </c>
+      <c r="D124" s="8">
+        <v>30</v>
+      </c>
+      <c r="E124" s="8">
+        <v>0</v>
+      </c>
+      <c r="F124" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G124" s="8">
+        <f>VLOOKUP($F124,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H124" s="8">
+        <f>VLOOKUP($F124,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I124" s="8">
+        <f t="shared" si="5"/>
+        <v>5.9415500000000003</v>
+      </c>
+      <c r="J124" s="8">
+        <f>VLOOKUP($F124,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K124" s="8">
+        <f>VLOOKUP($F124,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="7">
+        <v>28</v>
+      </c>
+      <c r="B125" s="7">
+        <v>19</v>
+      </c>
+      <c r="C125" s="8">
+        <v>10</v>
+      </c>
+      <c r="D125" s="8">
+        <v>30</v>
+      </c>
+      <c r="E125" s="8">
+        <v>0</v>
+      </c>
+      <c r="F125" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G125" s="8">
+        <f>VLOOKUP($F125,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H125" s="8">
+        <f>VLOOKUP($F125,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I125" s="8">
+        <f t="shared" si="5"/>
+        <v>9.9415499999999994</v>
+      </c>
+      <c r="J125" s="8">
+        <f>VLOOKUP($F125,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K125" s="8">
+        <f>VLOOKUP($F125,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="7">
+        <v>21</v>
+      </c>
+      <c r="B126" s="7">
+        <v>20</v>
+      </c>
+      <c r="C126" s="8">
+        <v>4</v>
+      </c>
+      <c r="D126" s="8">
+        <v>30</v>
+      </c>
+      <c r="E126" s="8">
+        <v>0</v>
+      </c>
+      <c r="F126" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G126" s="8">
+        <f>VLOOKUP($F126,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H126" s="8">
+        <f>VLOOKUP($F126,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I126" s="8">
+        <f t="shared" si="5"/>
+        <v>3.9415499999999999</v>
+      </c>
+      <c r="J126" s="8">
+        <f>VLOOKUP($F126,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K126" s="8">
+        <f>VLOOKUP($F126,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="7">
+        <v>28</v>
+      </c>
+      <c r="B127" s="7">
+        <v>21</v>
+      </c>
+      <c r="C127" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="D127" s="8">
+        <v>30</v>
+      </c>
+      <c r="E127" s="8">
+        <v>0</v>
+      </c>
+      <c r="F127" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G127" s="8">
+        <f>VLOOKUP($F127,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H127" s="8">
+        <f>VLOOKUP($F127,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I127" s="8">
+        <f t="shared" si="5"/>
+        <v>6.4415500000000003</v>
+      </c>
+      <c r="J127" s="8">
+        <f>VLOOKUP($F127,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K127" s="8">
+        <f>VLOOKUP($F127,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="7">
+        <v>26</v>
+      </c>
+      <c r="B128" s="7">
+        <v>22</v>
+      </c>
+      <c r="C128" s="8">
+        <v>15</v>
+      </c>
+      <c r="D128" s="8">
+        <v>80</v>
+      </c>
+      <c r="E128" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F128" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G128" s="8">
+        <f>VLOOKUP($F128,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H128" s="8">
+        <f>VLOOKUP($F128,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I128" s="8">
+        <f t="shared" si="5"/>
+        <v>14.58432</v>
+      </c>
+      <c r="J128" s="8">
+        <f>VLOOKUP($F128,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K128" s="8">
+        <f>VLOOKUP($F128,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="7">
+        <v>21</v>
+      </c>
+      <c r="B129" s="7">
+        <v>23</v>
+      </c>
+      <c r="C129" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="D129" s="8">
+        <v>30</v>
+      </c>
+      <c r="E129" s="8">
+        <v>0</v>
+      </c>
+      <c r="F129" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G129" s="8">
+        <f>VLOOKUP($F129,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H129" s="8">
+        <f>VLOOKUP($F129,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I129" s="8">
+        <f t="shared" si="5"/>
+        <v>4.4415500000000003</v>
+      </c>
+      <c r="J129" s="8">
+        <f>VLOOKUP($F129,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K129" s="8">
+        <f>VLOOKUP($F129,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="7">
+        <v>24</v>
+      </c>
+      <c r="B130" s="7">
+        <v>23</v>
+      </c>
+      <c r="C130" s="8">
+        <v>7</v>
+      </c>
+      <c r="D130" s="8">
+        <v>30</v>
+      </c>
+      <c r="E130" s="8">
+        <v>0</v>
+      </c>
+      <c r="F130" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G130" s="8">
+        <f>VLOOKUP($F130,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H130" s="8">
+        <f>VLOOKUP($F130,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I130" s="8">
+        <f t="shared" si="5"/>
+        <v>6.9415500000000003</v>
+      </c>
+      <c r="J130" s="8">
+        <f>VLOOKUP($F130,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K130" s="8">
+        <f>VLOOKUP($F130,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="7">
+        <v>20</v>
+      </c>
+      <c r="B131" s="7">
+        <v>24</v>
+      </c>
+      <c r="C131" s="8">
+        <v>11</v>
+      </c>
+      <c r="D131" s="8">
+        <v>30</v>
+      </c>
+      <c r="E131" s="8">
+        <v>0</v>
+      </c>
+      <c r="F131" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G131" s="8">
+        <f>VLOOKUP($F131,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H131" s="8">
+        <f>VLOOKUP($F131,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I131" s="8">
+        <f t="shared" si="5"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J131" s="8">
+        <f>VLOOKUP($F131,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K131" s="8">
+        <f>VLOOKUP($F131,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="7">
+        <v>22</v>
+      </c>
+      <c r="B132" s="7">
+        <v>24</v>
+      </c>
+      <c r="C132" s="8">
+        <v>15</v>
+      </c>
+      <c r="D132" s="8">
+        <v>30</v>
+      </c>
+      <c r="E132" s="8">
+        <v>0</v>
+      </c>
+      <c r="F132" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G132" s="8">
+        <f>VLOOKUP($F132,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H132" s="8">
+        <f>VLOOKUP($F132,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I132" s="8">
+        <f t="shared" si="5"/>
+        <v>14.941549999999999</v>
+      </c>
+      <c r="J132" s="8">
+        <f>VLOOKUP($F132,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K132" s="8">
+        <f>VLOOKUP($F132,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="7">
+        <v>26</v>
+      </c>
+      <c r="B133" s="7">
+        <v>24</v>
+      </c>
+      <c r="C133" s="8">
+        <v>11</v>
+      </c>
+      <c r="D133" s="8">
+        <v>30</v>
+      </c>
+      <c r="E133" s="8">
+        <v>0</v>
+      </c>
+      <c r="F133" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G133" s="8">
+        <f>VLOOKUP($F133,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H133" s="8">
+        <f>VLOOKUP($F133,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I133" s="8">
+        <f t="shared" si="5"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J133" s="8">
+        <f>VLOOKUP($F133,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K133" s="8">
+        <f>VLOOKUP($F133,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="7">
+        <v>24</v>
+      </c>
+      <c r="B134" s="7">
+        <v>25</v>
+      </c>
+      <c r="C134" s="8">
+        <v>5</v>
+      </c>
+      <c r="D134" s="8">
+        <v>30</v>
+      </c>
+      <c r="E134" s="8">
+        <v>0</v>
+      </c>
+      <c r="F134" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G134" s="8">
+        <f>VLOOKUP($F134,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H134" s="8">
+        <f>VLOOKUP($F134,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I134" s="8">
+        <f t="shared" si="5"/>
+        <v>4.9415500000000003</v>
+      </c>
+      <c r="J134" s="8">
+        <f>VLOOKUP($F134,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K134" s="8">
+        <f>VLOOKUP($F134,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="7">
+        <v>26</v>
+      </c>
+      <c r="B135" s="7">
+        <v>25</v>
+      </c>
+      <c r="C135" s="8">
+        <v>10</v>
+      </c>
+      <c r="D135" s="8">
+        <v>50</v>
+      </c>
+      <c r="E135" s="8">
+        <v>0</v>
+      </c>
+      <c r="F135" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G135" s="8">
+        <f>VLOOKUP($F135,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H135" s="8">
+        <f>VLOOKUP($F135,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I135" s="8">
+        <f t="shared" si="5"/>
+        <v>9.8376199999999994</v>
+      </c>
+      <c r="J135" s="8">
+        <f>VLOOKUP($F135,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K135" s="8">
+        <f>VLOOKUP($F135,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="7">
+        <v>27</v>
+      </c>
+      <c r="B136" s="7">
+        <v>25</v>
+      </c>
+      <c r="C136" s="8">
+        <v>14</v>
+      </c>
+      <c r="D136" s="8">
+        <v>50</v>
+      </c>
+      <c r="E136" s="8">
+        <v>0</v>
+      </c>
+      <c r="F136" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G136" s="8">
+        <f>VLOOKUP($F136,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H136" s="8">
+        <f>VLOOKUP($F136,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I136" s="8">
+        <f t="shared" si="5"/>
+        <v>13.837619999999999</v>
+      </c>
+      <c r="J136" s="8">
+        <f>VLOOKUP($F136,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K136" s="8">
+        <f>VLOOKUP($F136,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="7">
+        <v>34</v>
+      </c>
+      <c r="B137" s="7">
+        <v>25</v>
+      </c>
+      <c r="C137" s="8">
+        <v>19</v>
+      </c>
+      <c r="D137" s="8">
+        <v>30</v>
+      </c>
+      <c r="E137" s="8">
+        <v>0</v>
+      </c>
+      <c r="F137" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G137" s="8">
+        <f>VLOOKUP($F137,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H137" s="8">
+        <f>VLOOKUP($F137,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I137" s="8">
+        <f t="shared" si="5"/>
+        <v>18.941549999999999</v>
+      </c>
+      <c r="J137" s="8">
+        <f>VLOOKUP($F137,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K137" s="8">
+        <f>VLOOKUP($F137,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="7">
+        <v>37</v>
+      </c>
+      <c r="B138" s="7">
+        <v>25</v>
+      </c>
+      <c r="C138" s="8">
+        <v>19</v>
+      </c>
+      <c r="D138" s="8">
+        <v>50</v>
+      </c>
+      <c r="E138" s="8">
+        <v>0</v>
+      </c>
+      <c r="F138" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G138" s="8">
+        <f>VLOOKUP($F138,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H138" s="8">
+        <f>VLOOKUP($F138,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I138" s="8">
+        <f t="shared" si="5"/>
+        <v>18.837620000000001</v>
+      </c>
+      <c r="J138" s="8">
+        <f>VLOOKUP($F138,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K138" s="8">
+        <f>VLOOKUP($F138,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="7">
+        <v>23</v>
+      </c>
+      <c r="B139" s="7">
+        <v>27</v>
+      </c>
+      <c r="C139" s="8">
+        <v>8</v>
+      </c>
+      <c r="D139" s="8">
+        <v>30</v>
+      </c>
+      <c r="E139" s="8">
+        <v>0</v>
+      </c>
+      <c r="F139" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G139" s="8">
+        <f>VLOOKUP($F139,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H139" s="8">
+        <f>VLOOKUP($F139,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I139" s="8">
+        <f t="shared" si="5"/>
+        <v>7.9415500000000003</v>
+      </c>
+      <c r="J139" s="8">
+        <f>VLOOKUP($F139,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K139" s="8">
+        <f>VLOOKUP($F139,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="7">
+        <v>28</v>
+      </c>
+      <c r="B140" s="7">
+        <v>27</v>
+      </c>
+      <c r="C140" s="8">
+        <v>3</v>
+      </c>
+      <c r="D140" s="8">
+        <v>50</v>
+      </c>
+      <c r="E140" s="8">
+        <v>0</v>
+      </c>
+      <c r="F140" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Main Type 1</v>
+      </c>
+      <c r="G140" s="8">
+        <f>VLOOKUP($F140,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>6.4944444444444442E-3</v>
+      </c>
+      <c r="H140" s="8">
+        <f>VLOOKUP($F140,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.16238</v>
+      </c>
+      <c r="I140" s="8">
+        <f t="shared" si="5"/>
+        <v>2.8376199999999998</v>
+      </c>
+      <c r="J140" s="8">
+        <f>VLOOKUP($F140,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>7.3019999999999996</v>
+      </c>
+      <c r="K140" s="8">
+        <f>VLOOKUP($F140,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>6.2399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="7">
+        <v>33</v>
+      </c>
+      <c r="B141" s="7">
+        <v>27</v>
+      </c>
+      <c r="C141" s="8">
+        <v>8</v>
+      </c>
+      <c r="D141" s="8">
+        <v>30</v>
+      </c>
+      <c r="E141" s="8">
+        <v>0</v>
+      </c>
+      <c r="F141" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G141" s="8">
+        <f>VLOOKUP($F141,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H141" s="8">
+        <f>VLOOKUP($F141,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I141" s="8">
+        <f t="shared" si="5"/>
+        <v>7.9415500000000003</v>
+      </c>
+      <c r="J141" s="8">
+        <f>VLOOKUP($F141,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K141" s="8">
+        <f>VLOOKUP($F141,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="7">
+        <v>35</v>
+      </c>
+      <c r="B142" s="7">
+        <v>27</v>
+      </c>
+      <c r="C142" s="8">
+        <v>7</v>
+      </c>
+      <c r="D142" s="8">
+        <v>30</v>
+      </c>
+      <c r="E142" s="8">
+        <v>0</v>
+      </c>
+      <c r="F142" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G142" s="8">
+        <f>VLOOKUP($F142,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H142" s="8">
+        <f>VLOOKUP($F142,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I142" s="8">
+        <f t="shared" si="5"/>
+        <v>6.9415500000000003</v>
+      </c>
+      <c r="J142" s="8">
+        <f>VLOOKUP($F142,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K142" s="8">
+        <f>VLOOKUP($F142,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="7">
+        <v>17</v>
+      </c>
+      <c r="B143" s="7">
+        <v>29</v>
+      </c>
+      <c r="C143" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D143" s="8">
+        <v>30</v>
+      </c>
+      <c r="E143" s="8">
+        <v>0</v>
+      </c>
+      <c r="F143" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G143" s="8">
+        <f>VLOOKUP($F143,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H143" s="8">
+        <f>VLOOKUP($F143,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I143" s="8">
+        <f t="shared" si="5"/>
+        <v>7.4415500000000003</v>
+      </c>
+      <c r="J143" s="8">
+        <f>VLOOKUP($F143,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K143" s="8">
+        <f>VLOOKUP($F143,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="7">
+        <v>27</v>
+      </c>
+      <c r="B144" s="7">
+        <v>29</v>
+      </c>
+      <c r="C144" s="8">
+        <v>9.5</v>
+      </c>
+      <c r="D144" s="8">
+        <v>30</v>
+      </c>
+      <c r="E144" s="8">
+        <v>0</v>
+      </c>
+      <c r="F144" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G144" s="8">
+        <f>VLOOKUP($F144,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H144" s="8">
+        <f>VLOOKUP($F144,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I144" s="8">
+        <f t="shared" si="5"/>
+        <v>9.4415499999999994</v>
+      </c>
+      <c r="J144" s="8">
+        <f>VLOOKUP($F144,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K144" s="8">
+        <f>VLOOKUP($F144,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="7">
+        <v>30</v>
+      </c>
+      <c r="B145" s="7">
+        <v>29</v>
+      </c>
+      <c r="C145" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D145" s="8">
+        <v>30</v>
+      </c>
+      <c r="E145" s="8">
+        <v>0</v>
+      </c>
+      <c r="F145" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G145" s="8">
+        <f>VLOOKUP($F145,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H145" s="8">
+        <f>VLOOKUP($F145,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I145" s="8">
+        <f t="shared" si="5"/>
+        <v>3.4415499999999999</v>
+      </c>
+      <c r="J145" s="8">
+        <f>VLOOKUP($F145,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K145" s="8">
+        <f>VLOOKUP($F145,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="7">
+        <v>33</v>
+      </c>
+      <c r="B146" s="7">
+        <v>29</v>
+      </c>
+      <c r="C146" s="8">
+        <v>6</v>
+      </c>
+      <c r="D146" s="8">
+        <v>30</v>
+      </c>
+      <c r="E146" s="8">
+        <v>0</v>
+      </c>
+      <c r="F146" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G146" s="8">
+        <f>VLOOKUP($F146,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H146" s="8">
+        <f>VLOOKUP($F146,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I146" s="8">
+        <f t="shared" si="5"/>
+        <v>5.9415500000000003</v>
+      </c>
+      <c r="J146" s="8">
+        <f>VLOOKUP($F146,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K146" s="8">
+        <f>VLOOKUP($F146,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="7">
+        <v>17</v>
+      </c>
+      <c r="B147" s="7">
+        <v>30</v>
+      </c>
+      <c r="C147" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D147" s="8">
+        <v>30</v>
+      </c>
+      <c r="E147" s="8">
+        <v>0</v>
+      </c>
+      <c r="F147" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G147" s="8">
+        <f>VLOOKUP($F147,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H147" s="8">
+        <f>VLOOKUP($F147,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I147" s="8">
+        <f t="shared" si="5"/>
+        <v>8.4415499999999994</v>
+      </c>
+      <c r="J147" s="8">
+        <f>VLOOKUP($F147,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K147" s="8">
+        <f>VLOOKUP($F147,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="7">
+        <v>31</v>
+      </c>
+      <c r="B148" s="7">
+        <v>30</v>
+      </c>
+      <c r="C148" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D148" s="8">
+        <v>30</v>
+      </c>
+      <c r="E148" s="8">
+        <v>0</v>
+      </c>
+      <c r="F148" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G148" s="8">
+        <f>VLOOKUP($F148,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H148" s="8">
+        <f>VLOOKUP($F148,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I148" s="8">
+        <f t="shared" si="5"/>
+        <v>3.4415499999999999</v>
+      </c>
+      <c r="J148" s="8">
+        <f>VLOOKUP($F148,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K148" s="8">
+        <f>VLOOKUP($F148,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="7">
+        <v>36</v>
+      </c>
+      <c r="B149" s="7">
+        <v>30</v>
+      </c>
+      <c r="C149" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D149" s="8">
+        <v>30</v>
+      </c>
+      <c r="E149" s="8">
+        <v>0</v>
+      </c>
+      <c r="F149" s="8" t="str">
+        <f t="shared" ref="F149:F163" si="6">IF(D149=30,"Secondary",IF(D149=50,"Main Type 1",IF(D149=80,"Main Type 2","Unknown")))</f>
+        <v>Secondary</v>
+      </c>
+      <c r="G149" s="8">
+        <f>VLOOKUP($F149,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H149" s="8">
+        <f>VLOOKUP($F149,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I149" s="8">
+        <f t="shared" ref="I149:I163" si="7">C149-H149</f>
+        <v>8.4415499999999994</v>
+      </c>
+      <c r="J149" s="8">
+        <f>VLOOKUP($F149,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K149" s="8">
+        <f>VLOOKUP($F149,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="7">
+        <v>36</v>
+      </c>
+      <c r="B150" s="7">
+        <v>31</v>
+      </c>
+      <c r="C150" s="8">
+        <v>10</v>
+      </c>
+      <c r="D150" s="8">
+        <v>80</v>
+      </c>
+      <c r="E150" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F150" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G150" s="8">
+        <f>VLOOKUP($F150,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H150" s="8">
+        <f>VLOOKUP($F150,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I150" s="8">
+        <f t="shared" si="7"/>
+        <v>9.58432</v>
+      </c>
+      <c r="J150" s="8">
+        <f>VLOOKUP($F150,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K150" s="8">
+        <f>VLOOKUP($F150,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="7">
+        <v>29</v>
+      </c>
+      <c r="B151" s="7">
+        <v>32</v>
+      </c>
+      <c r="C151" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="D151" s="8">
+        <v>30</v>
+      </c>
+      <c r="E151" s="8">
+        <v>0</v>
+      </c>
+      <c r="F151" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G151" s="8">
+        <f>VLOOKUP($F151,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H151" s="8">
+        <f>VLOOKUP($F151,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I151" s="8">
+        <f t="shared" si="7"/>
+        <v>2.3415499999999998</v>
+      </c>
+      <c r="J151" s="8">
+        <f>VLOOKUP($F151,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K151" s="8">
+        <f>VLOOKUP($F151,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="7">
+        <v>32</v>
+      </c>
+      <c r="B152" s="7">
+        <v>33</v>
+      </c>
+      <c r="C152" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D152" s="8">
+        <v>30</v>
+      </c>
+      <c r="E152" s="8">
+        <v>0</v>
+      </c>
+      <c r="F152" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G152" s="8">
+        <f>VLOOKUP($F152,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H152" s="8">
+        <f>VLOOKUP($F152,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I152" s="8">
+        <f t="shared" si="7"/>
+        <v>3.4415499999999999</v>
+      </c>
+      <c r="J152" s="8">
+        <f>VLOOKUP($F152,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K152" s="8">
+        <f>VLOOKUP($F152,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="7">
+        <v>35</v>
+      </c>
+      <c r="B153" s="7">
+        <v>33</v>
+      </c>
+      <c r="C153" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D153" s="8">
+        <v>30</v>
+      </c>
+      <c r="E153" s="8">
+        <v>0</v>
+      </c>
+      <c r="F153" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G153" s="8">
+        <f>VLOOKUP($F153,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H153" s="8">
+        <f>VLOOKUP($F153,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I153" s="8">
+        <f t="shared" si="7"/>
+        <v>3.4415499999999999</v>
+      </c>
+      <c r="J153" s="8">
+        <f>VLOOKUP($F153,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K153" s="8">
+        <f>VLOOKUP($F153,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="7">
+        <v>27</v>
+      </c>
+      <c r="B154" s="7">
+        <v>34</v>
+      </c>
+      <c r="C154" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D154" s="8">
+        <v>30</v>
+      </c>
+      <c r="E154" s="8">
+        <v>0</v>
+      </c>
+      <c r="F154" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G154" s="8">
+        <f>VLOOKUP($F154,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H154" s="8">
+        <f>VLOOKUP($F154,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I154" s="8">
+        <f t="shared" si="7"/>
+        <v>7.4415500000000003</v>
+      </c>
+      <c r="J154" s="8">
+        <f>VLOOKUP($F154,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K154" s="8">
+        <f>VLOOKUP($F154,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="7">
+        <v>35</v>
+      </c>
+      <c r="B155" s="7">
+        <v>34</v>
+      </c>
+      <c r="C155" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="D155" s="8">
+        <v>30</v>
+      </c>
+      <c r="E155" s="8">
+        <v>0</v>
+      </c>
+      <c r="F155" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G155" s="8">
+        <f>VLOOKUP($F155,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H155" s="8">
+        <f>VLOOKUP($F155,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I155" s="8">
+        <f t="shared" si="7"/>
+        <v>4.4415500000000003</v>
+      </c>
+      <c r="J155" s="8">
+        <f>VLOOKUP($F155,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K155" s="8">
+        <f>VLOOKUP($F155,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="7">
+        <v>36</v>
+      </c>
+      <c r="B156" s="7">
+        <v>35</v>
+      </c>
+      <c r="C156" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="D156" s="8">
+        <v>30</v>
+      </c>
+      <c r="E156" s="8">
+        <v>0</v>
+      </c>
+      <c r="F156" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G156" s="8">
+        <f>VLOOKUP($F156,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H156" s="8">
+        <f>VLOOKUP($F156,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I156" s="8">
+        <f t="shared" si="7"/>
+        <v>6.4415500000000003</v>
+      </c>
+      <c r="J156" s="8">
+        <f>VLOOKUP($F156,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K156" s="8">
+        <f>VLOOKUP($F156,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="7">
+        <v>32</v>
+      </c>
+      <c r="B157" s="7">
+        <v>36</v>
+      </c>
+      <c r="C157" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D157" s="8">
+        <v>30</v>
+      </c>
+      <c r="E157" s="8">
+        <v>0</v>
+      </c>
+      <c r="F157" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G157" s="8">
+        <f>VLOOKUP($F157,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H157" s="8">
+        <f>VLOOKUP($F157,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I157" s="8">
+        <f t="shared" si="7"/>
+        <v>8.4415499999999994</v>
+      </c>
+      <c r="J157" s="8">
+        <f>VLOOKUP($F157,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K157" s="8">
+        <f>VLOOKUP($F157,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="7">
+        <v>37</v>
+      </c>
+      <c r="B158" s="7">
+        <v>36</v>
+      </c>
+      <c r="C158" s="8">
+        <v>8</v>
+      </c>
+      <c r="D158" s="8">
+        <v>80</v>
+      </c>
+      <c r="E158" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="F158" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Main Type 2</v>
+      </c>
+      <c r="G158" s="8">
+        <f>VLOOKUP($F158,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>1.0391666666666665E-2</v>
+      </c>
+      <c r="H158" s="8">
+        <f>VLOOKUP($F158,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>0.41567999999999999</v>
+      </c>
+      <c r="I158" s="8">
+        <f t="shared" si="7"/>
+        <v>7.58432</v>
+      </c>
+      <c r="J158" s="8">
+        <f>VLOOKUP($F158,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>15.19</v>
+      </c>
+      <c r="K158" s="8">
+        <f>VLOOKUP($F158,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="7">
+        <v>34</v>
+      </c>
+      <c r="B159" s="7">
+        <v>37</v>
+      </c>
+      <c r="C159" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="D159" s="8">
+        <v>30</v>
+      </c>
+      <c r="E159" s="8">
+        <v>0</v>
+      </c>
+      <c r="F159" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G159" s="8">
+        <f>VLOOKUP($F159,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H159" s="8">
+        <f>VLOOKUP($F159,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I159" s="8">
+        <f t="shared" si="7"/>
+        <v>6.4415500000000003</v>
+      </c>
+      <c r="J159" s="8">
+        <f>VLOOKUP($F159,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K159" s="8">
+        <f>VLOOKUP($F159,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="7">
+        <v>35</v>
+      </c>
+      <c r="B160" s="7">
+        <v>37</v>
+      </c>
+      <c r="C160" s="8">
+        <v>7</v>
+      </c>
+      <c r="D160" s="8">
+        <v>30</v>
+      </c>
+      <c r="E160" s="8">
+        <v>0</v>
+      </c>
+      <c r="F160" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G160" s="8">
+        <f>VLOOKUP($F160,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H160" s="8">
+        <f>VLOOKUP($F160,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I160" s="8">
+        <f t="shared" si="7"/>
+        <v>6.9415500000000003</v>
+      </c>
+      <c r="J160" s="8">
+        <f>VLOOKUP($F160,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K160" s="8">
+        <f>VLOOKUP($F160,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="7">
+        <v>20</v>
+      </c>
+      <c r="B161" s="7">
+        <v>38</v>
+      </c>
+      <c r="C161" s="8">
+        <v>11</v>
+      </c>
+      <c r="D161" s="8">
+        <v>30</v>
+      </c>
+      <c r="E161" s="8">
+        <v>0</v>
+      </c>
+      <c r="F161" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G161" s="8">
+        <f>VLOOKUP($F161,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H161" s="8">
+        <f>VLOOKUP($F161,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I161" s="8">
+        <f t="shared" si="7"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J161" s="8">
+        <f>VLOOKUP($F161,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K161" s="8">
+        <f>VLOOKUP($F161,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="7">
+        <v>22</v>
+      </c>
+      <c r="B162" s="7">
+        <v>38</v>
+      </c>
+      <c r="C162" s="8">
+        <v>15</v>
+      </c>
+      <c r="D162" s="8">
+        <v>30</v>
+      </c>
+      <c r="E162" s="8">
+        <v>0</v>
+      </c>
+      <c r="F162" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G162" s="8">
+        <f>VLOOKUP($F162,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H162" s="8">
+        <f>VLOOKUP($F162,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I162" s="8">
+        <f t="shared" si="7"/>
+        <v>14.941549999999999</v>
+      </c>
+      <c r="J162" s="8">
+        <f>VLOOKUP($F162,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K162" s="8">
+        <f>VLOOKUP($F162,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="7">
+        <v>26</v>
+      </c>
+      <c r="B163" s="7">
+        <v>38</v>
+      </c>
+      <c r="C163" s="8">
+        <v>11</v>
+      </c>
+      <c r="D163" s="8">
+        <v>30</v>
+      </c>
+      <c r="E163" s="8">
+        <v>0</v>
+      </c>
+      <c r="F163" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Secondary</v>
+      </c>
+      <c r="G163" s="8">
+        <f>VLOOKUP($F163,sPathTypes!$A:$I,6,FALSE)</f>
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H163" s="8">
+        <f>VLOOKUP($F163,sPathTypes!$A:$I,7,FALSE)</f>
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I163" s="8">
+        <f t="shared" si="7"/>
+        <v>10.941549999999999</v>
+      </c>
+      <c r="J163" s="8">
+        <f>VLOOKUP($F163,sPathTypes!$A:$I,8,FALSE)</f>
+        <v>4.444</v>
+      </c>
+      <c r="K163" s="8">
+        <f>VLOOKUP($F163,sPathTypes!$A:$I,9,FALSE)</f>
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="7">
+        <v>38</v>
+      </c>
+      <c r="B164" s="7">
+        <v>23</v>
+      </c>
+      <c r="C164" s="8">
+        <v>7</v>
+      </c>
+      <c r="D164" s="8">
+        <v>30</v>
+      </c>
+      <c r="E164" s="8">
+        <v>0</v>
+      </c>
+      <c r="F164" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G164" s="8">
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H164" s="8">
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I164" s="8">
+        <v>6.9415500000000003</v>
+      </c>
+      <c r="J164" s="8">
+        <v>4.444</v>
+      </c>
+      <c r="K164" s="8">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="7">
+        <v>38</v>
+      </c>
+      <c r="B165" s="7">
+        <v>25</v>
+      </c>
+      <c r="C165" s="8">
+        <v>5</v>
+      </c>
+      <c r="D165" s="8">
+        <v>30</v>
+      </c>
+      <c r="E165" s="8">
+        <v>0</v>
+      </c>
+      <c r="F165" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G165" s="8">
+        <v>3.8972222222222225E-3</v>
+      </c>
+      <c r="H165" s="8">
+        <v>5.8450000000000002E-2</v>
+      </c>
+      <c r="I165" s="8">
+        <v>4.9415500000000003</v>
+      </c>
+      <c r="J165" s="8">
+        <v>4.444</v>
+      </c>
+      <c r="K165" s="8">
         <v>2.24E-2</v>
       </c>
     </row>
@@ -4188,10 +7551,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="A5" sqref="A5:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4237,7 +7601,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4254,7 +7618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4288,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -4305,7 +7669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -4339,7 +7703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -4356,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -4391,7 +7755,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -4408,7 +7772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>3</v>
       </c>
@@ -4442,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -4460,7 +7824,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E15" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E15" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>